<commit_message>
Aanwezigheid, scale & time
Aanwezigheid scales en times zijn geupdate
</commit_message>
<xml_diff>
--- a/Aanwezigheid.xlsx
+++ b/Aanwezigheid.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="21075" windowHeight="8520"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="21075" windowHeight="8520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Aanwezigheid" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="59">
   <si>
     <t>Maandag</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>in unity</t>
+  </si>
+  <si>
+    <t>Rotatie om as in graden per seconde</t>
   </si>
 </sst>
 </file>
@@ -308,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -318,6 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -641,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +702,7 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>54</v>
       </c>
       <c r="J3" t="s">
@@ -727,7 +731,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="I4" s="9"/>
+      <c r="I4" s="10"/>
       <c r="J4" t="s">
         <v>1</v>
       </c>
@@ -752,7 +756,7 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="I5" s="9"/>
+      <c r="I5" s="10"/>
       <c r="J5" t="s">
         <v>2</v>
       </c>
@@ -777,10 +781,15 @@
         <v>15</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="I6" s="9"/>
+      <c r="I6" s="10"/>
       <c r="J6" t="s">
         <v>3</v>
       </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
       <c r="Q6" t="s">
         <v>13</v>
       </c>
@@ -849,7 +858,7 @@
       <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B10" t="s">
@@ -867,7 +876,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -881,7 +890,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="10"/>
       <c r="B12" t="s">
         <v>2</v>
       </c>
@@ -895,7 +904,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -1238,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C8:T42"/>
+  <dimension ref="C8:T54"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,24 +1263,24 @@
   </cols>
   <sheetData>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="12" t="s">
+      <c r="G8" s="11"/>
+      <c r="H8" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="10" t="s">
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
       <c r="S8" t="s">
         <v>39</v>
       </c>
@@ -1280,24 +1289,24 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="11">
         <v>57900000000</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11">
         <v>4878000</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="12">
+      <c r="G9" s="11"/>
+      <c r="H9" s="13">
         <v>88</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="10">
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="11">
         <v>58.6</v>
       </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
       <c r="S9" t="s">
         <v>40</v>
       </c>
@@ -1306,24 +1315,24 @@
       <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="11">
         <v>108200000000</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11">
         <v>12104000</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="12">
+      <c r="G10" s="11"/>
+      <c r="H10" s="13">
         <v>225</v>
       </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="10">
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="11">
         <v>241</v>
       </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
       <c r="S10" t="s">
         <v>41</v>
       </c>
@@ -1332,24 +1341,24 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="11">
         <v>149600000000</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11">
         <v>12760000</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="12">
+      <c r="G11" s="11"/>
+      <c r="H11" s="13">
         <v>365.24</v>
       </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="10">
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="11">
         <v>1</v>
       </c>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
       <c r="S11" t="s">
         <v>42</v>
       </c>
@@ -1358,28 +1367,28 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="12">
         <v>227900000000</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11">
+      <c r="E12" s="12"/>
+      <c r="F12" s="12">
         <v>6787000</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="13">
+      <c r="G12" s="12"/>
+      <c r="H12" s="14">
         <v>687</v>
       </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="11">
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="12">
         <v>1.02</v>
       </c>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="P12" s="14" t="s">
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="P12" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="Q12" s="15"/>
+      <c r="Q12" s="16"/>
       <c r="S12" t="s">
         <v>43</v>
       </c>
@@ -1388,29 +1397,29 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="12">
         <v>778300000000</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11">
+      <c r="E13" s="12"/>
+      <c r="F13" s="12">
         <v>139822000</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="13">
+      <c r="G13" s="12"/>
+      <c r="H13" s="14">
         <v>4343.5</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="11">
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="12">
         <v>0.41</v>
       </c>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="P13" s="16">
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="P13" s="17">
         <f>F11*10</f>
         <v>127600000</v>
       </c>
-      <c r="Q13" s="16"/>
+      <c r="Q13" s="17"/>
       <c r="S13" t="s">
         <v>44</v>
       </c>
@@ -1419,280 +1428,280 @@
       <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="12">
         <v>1427000000000</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12">
         <v>120500000</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="13">
+      <c r="G14" s="12"/>
+      <c r="H14" s="14">
         <v>10767.5</v>
       </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="11">
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="12">
         <v>0.44</v>
       </c>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="12">
         <v>2871000000000</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11">
+      <c r="E15" s="12"/>
+      <c r="F15" s="12">
         <v>51120000</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="13">
+      <c r="G15" s="12"/>
+      <c r="H15" s="14">
         <v>30660</v>
       </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="11">
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="12">
         <v>0.75</v>
       </c>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="12">
         <v>4497100000000</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12">
         <v>49530000</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="13">
+      <c r="G16" s="12"/>
+      <c r="H16" s="14">
         <v>60225</v>
       </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="11">
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="12">
         <v>0.79</v>
       </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="12">
         <v>5913000000000</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12">
         <v>2301000</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="13">
+      <c r="G17" s="12"/>
+      <c r="H17" s="14">
         <v>90520</v>
       </c>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="11">
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="12">
         <v>6.4</v>
       </c>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11">
+      <c r="E18" s="11"/>
+      <c r="F18" s="12">
         <v>1391000000</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="12" t="s">
+      <c r="G18" s="12"/>
+      <c r="H18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="11">
+        <v>27</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10" t="s">
+      <c r="E20" s="11"/>
+      <c r="F20" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="12" t="s">
+      <c r="G20" s="11"/>
+      <c r="H20" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="10" t="s">
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="P20" s="17" t="s">
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="P20" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="Q20" s="17"/>
+      <c r="Q20" s="18"/>
     </row>
     <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="11">
         <f>D9/$P$13</f>
         <v>453.76175548589339</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10">
+      <c r="E21" s="11"/>
+      <c r="F21" s="11">
         <f>F9/$P$13</f>
         <v>3.822884012539185E-2</v>
       </c>
-      <c r="G21" s="10"/>
-      <c r="H21" s="12">
+      <c r="G21" s="11"/>
+      <c r="H21" s="13">
         <f>((H9*24)*60)*60</f>
         <v>7603200</v>
       </c>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12">
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13">
         <f>((K9*24)*60)*60</f>
         <v>5063040</v>
       </c>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="P21" s="18">
-        <f>H21/30</f>
-        <v>253440</v>
-      </c>
-      <c r="Q21" s="18"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="P21" s="19">
+        <f>K23/30</f>
+        <v>2880</v>
+      </c>
+      <c r="Q21" s="19"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="11">
         <f t="shared" ref="D22:D29" si="0">D10/$P$13</f>
         <v>847.96238244514109</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10">
+      <c r="E22" s="11"/>
+      <c r="F22" s="11">
         <f t="shared" ref="F22:F30" si="1">F10/$P$13</f>
         <v>9.4858934169278999E-2</v>
       </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="12">
+      <c r="G22" s="11"/>
+      <c r="H22" s="13">
         <f t="shared" ref="H22:H29" si="2">((H10*24)*60)*60</f>
         <v>19440000</v>
       </c>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12">
-        <f t="shared" ref="K22:K29" si="3">((K10*24)*60)*60</f>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13">
+        <f t="shared" ref="K22:K30" si="3">((K10*24)*60)*60</f>
         <v>20822400</v>
       </c>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
     </row>
     <row r="23" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="11">
         <f t="shared" si="0"/>
         <v>1172.4137931034484</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10">
+      <c r="E23" s="11"/>
+      <c r="F23" s="11">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="12">
+      <c r="G23" s="11"/>
+      <c r="H23" s="13">
         <f t="shared" si="2"/>
         <v>31556736</v>
       </c>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12">
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13">
         <f t="shared" si="3"/>
         <v>86400</v>
       </c>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="11">
         <f t="shared" si="0"/>
         <v>1786.0501567398119</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10">
+      <c r="E24" s="11"/>
+      <c r="F24" s="11">
         <f t="shared" si="1"/>
         <v>5.3189655172413794E-2</v>
       </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="12">
+      <c r="G24" s="11"/>
+      <c r="H24" s="13">
         <f t="shared" si="2"/>
         <v>59356800</v>
       </c>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12">
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13">
         <f t="shared" si="3"/>
         <v>88128</v>
       </c>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="11">
         <f t="shared" si="0"/>
         <v>6099.5297805642631</v>
       </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10">
+      <c r="E25" s="11"/>
+      <c r="F25" s="11">
         <f t="shared" si="1"/>
         <v>1.0957836990595611</v>
       </c>
-      <c r="G25" s="10"/>
-      <c r="H25" s="12">
+      <c r="G25" s="11"/>
+      <c r="H25" s="13">
         <f t="shared" si="2"/>
         <v>375278400</v>
       </c>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12">
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13">
         <f t="shared" si="3"/>
         <v>35424</v>
       </c>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
       <c r="Q25" t="s">
         <v>56</v>
       </c>
@@ -1704,28 +1713,28 @@
       <c r="C26" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="11">
         <f t="shared" si="0"/>
         <v>11183.385579937303</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10">
+      <c r="E26" s="11"/>
+      <c r="F26" s="11">
         <f t="shared" si="1"/>
         <v>0.94435736677115989</v>
       </c>
-      <c r="G26" s="10"/>
-      <c r="H26" s="12">
+      <c r="G26" s="11"/>
+      <c r="H26" s="13">
         <f t="shared" si="2"/>
         <v>930312000</v>
       </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12">
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13">
         <f t="shared" si="3"/>
         <v>38016</v>
       </c>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
       <c r="P26" t="s">
         <v>55</v>
       </c>
@@ -1741,259 +1750,416 @@
       <c r="C27" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="11">
         <f t="shared" si="0"/>
         <v>22500</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10">
+      <c r="E27" s="11"/>
+      <c r="F27" s="11">
         <f t="shared" si="1"/>
         <v>0.40062695924764891</v>
       </c>
-      <c r="G27" s="10"/>
-      <c r="H27" s="12">
+      <c r="G27" s="11"/>
+      <c r="H27" s="13">
         <f t="shared" si="2"/>
         <v>2649024000</v>
       </c>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12">
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13">
         <f t="shared" si="3"/>
         <v>64800</v>
       </c>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="11">
         <f t="shared" si="0"/>
         <v>35243.730407523508</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10">
+      <c r="E28" s="11"/>
+      <c r="F28" s="11">
         <f t="shared" si="1"/>
         <v>0.38816614420062695</v>
       </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="12">
+      <c r="G28" s="11"/>
+      <c r="H28" s="13">
         <f t="shared" si="2"/>
         <v>5203440000</v>
       </c>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12">
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13">
         <f t="shared" si="3"/>
         <v>68256.000000000015</v>
       </c>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="11">
         <f t="shared" si="0"/>
         <v>46340.125391849528</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10">
+      <c r="E29" s="11"/>
+      <c r="F29" s="11">
         <f t="shared" si="1"/>
         <v>1.8032915360501566E-2</v>
       </c>
-      <c r="G29" s="10"/>
-      <c r="H29" s="12">
+      <c r="G29" s="11"/>
+      <c r="H29" s="13">
         <f t="shared" si="2"/>
         <v>7820928000</v>
       </c>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12">
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13">
         <f t="shared" si="3"/>
         <v>552960.00000000012</v>
       </c>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10">
+      <c r="E30" s="11"/>
+      <c r="F30" s="11">
         <f t="shared" si="1"/>
         <v>10.901253918495298</v>
       </c>
-      <c r="G30" s="10"/>
-      <c r="H30" s="12" t="s">
+      <c r="G30" s="11"/>
+      <c r="H30" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="10" t="s">
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13">
+        <f t="shared" si="3"/>
+        <v>2332800</v>
+      </c>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="H32" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+    </row>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="13">
+        <f>H21/$P$21</f>
+        <v>2640</v>
+      </c>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13">
+        <f>K21/$P$21</f>
+        <v>1758</v>
+      </c>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+    </row>
+    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C34" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="13">
+        <f t="shared" ref="H34:H41" si="4">H22/$P$21</f>
+        <v>6750</v>
+      </c>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13">
+        <f t="shared" ref="K34:K42" si="5">K22/$P$21</f>
+        <v>7230</v>
+      </c>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+    </row>
+    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C35" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="13">
+        <f t="shared" si="4"/>
+        <v>10957.2</v>
+      </c>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+    </row>
+    <row r="36" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C36" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="13">
+        <f t="shared" si="4"/>
+        <v>20610</v>
+      </c>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13">
+        <f t="shared" si="5"/>
+        <v>30.6</v>
+      </c>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+    </row>
+    <row r="37" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C37" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" s="13">
+        <f t="shared" si="4"/>
+        <v>130305</v>
+      </c>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13">
+        <f t="shared" si="5"/>
+        <v>12.3</v>
+      </c>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C38" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="13">
+        <f t="shared" si="4"/>
+        <v>323025</v>
+      </c>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13">
+        <f t="shared" si="5"/>
+        <v>13.2</v>
+      </c>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C39" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" s="13">
+        <f t="shared" si="4"/>
+        <v>919800</v>
+      </c>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13">
+        <f t="shared" si="5"/>
+        <v>22.5</v>
+      </c>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+    </row>
+    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C40" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H40" s="13">
+        <f t="shared" si="4"/>
+        <v>1806750</v>
+      </c>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13">
+        <f t="shared" si="5"/>
+        <v>23.700000000000006</v>
+      </c>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+    </row>
+    <row r="41" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C41" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H41" s="13">
+        <f t="shared" si="4"/>
+        <v>2715600</v>
+      </c>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13">
+        <f t="shared" si="5"/>
+        <v>192.00000000000003</v>
+      </c>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+    </row>
+    <row r="42" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C42" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H42" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-    </row>
-    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="H32" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-    </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H33" s="12">
-        <f>H21/$P$21</f>
-        <v>30</v>
-      </c>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12">
-        <f>K21/$P$21</f>
-        <v>19.977272727272727</v>
-      </c>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-    </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H34" s="12">
-        <f t="shared" ref="H34:H41" si="4">H22/$P$21</f>
-        <v>76.704545454545453</v>
-      </c>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12">
-        <f t="shared" ref="K34:K41" si="5">K22/$P$21</f>
-        <v>82.159090909090907</v>
-      </c>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-    </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H35" s="12">
-        <f t="shared" si="4"/>
-        <v>124.51363636363637</v>
-      </c>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12">
-        <f t="shared" si="5"/>
-        <v>0.34090909090909088</v>
-      </c>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-    </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H36" s="12">
-        <f t="shared" si="4"/>
-        <v>234.20454545454547</v>
-      </c>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12">
-        <f t="shared" si="5"/>
-        <v>0.34772727272727272</v>
-      </c>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-    </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H37" s="12">
-        <f t="shared" si="4"/>
-        <v>1480.7386363636363</v>
-      </c>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12">
-        <f t="shared" si="5"/>
-        <v>0.13977272727272727</v>
-      </c>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-    </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H38" s="12">
-        <f t="shared" si="4"/>
-        <v>3670.7386363636365</v>
-      </c>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12">
-        <f t="shared" si="5"/>
-        <v>0.15</v>
-      </c>
-      <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-    </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H39" s="12">
-        <f t="shared" si="4"/>
-        <v>10452.272727272728</v>
-      </c>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12">
-        <f t="shared" si="5"/>
-        <v>0.25568181818181818</v>
-      </c>
-      <c r="L39" s="12"/>
-      <c r="M39" s="12"/>
-    </row>
-    <row r="40" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H40" s="12">
-        <f t="shared" si="4"/>
-        <v>20531.25</v>
-      </c>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12">
-        <f t="shared" si="5"/>
-        <v>0.2693181818181819</v>
-      </c>
-      <c r="L40" s="12"/>
-      <c r="M40" s="12"/>
-    </row>
-    <row r="41" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H41" s="12">
-        <f t="shared" si="4"/>
-        <v>30859.090909090908</v>
-      </c>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12">
-        <f t="shared" si="5"/>
-        <v>2.1818181818181821</v>
-      </c>
-      <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-    </row>
-    <row r="42" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H42" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13">
+        <f>K30/$P$21</f>
+        <v>810</v>
+      </c>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+    </row>
+    <row r="44" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="J45" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K45" s="11">
+        <f>360/K33</f>
+        <v>0.20477815699658702</v>
+      </c>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+    </row>
+    <row r="46" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="J46" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K46" s="11">
+        <f t="shared" ref="K46:K54" si="6">360/K34</f>
+        <v>4.9792531120331947E-2</v>
+      </c>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+    </row>
+    <row r="47" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="J47" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K47" s="11">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+    </row>
+    <row r="48" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="J48" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K48" s="11">
+        <f t="shared" si="6"/>
+        <v>11.76470588235294</v>
+      </c>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+    </row>
+    <row r="49" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J49" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K49" s="11">
+        <f t="shared" si="6"/>
+        <v>29.268292682926827</v>
+      </c>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+    </row>
+    <row r="50" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J50" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K50" s="11">
+        <f t="shared" si="6"/>
+        <v>27.272727272727273</v>
+      </c>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+    </row>
+    <row r="51" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J51" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K51" s="11">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+    </row>
+    <row r="52" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J52" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K52" s="11">
+        <f t="shared" si="6"/>
+        <v>15.189873417721515</v>
+      </c>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+    </row>
+    <row r="53" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J53" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K53" s="11">
+        <f t="shared" si="6"/>
+        <v>1.8749999999999998</v>
+      </c>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+    </row>
+    <row r="54" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K54" s="11">
+        <f>360/K42</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="114">
+  <mergeCells count="124">
+    <mergeCell ref="K54:M54"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="K46:M46"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="K50:M50"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="K52:M52"/>
+    <mergeCell ref="K53:M53"/>
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="K40:M40"/>
     <mergeCell ref="H41:J41"/>
@@ -2075,24 +2241,10 @@
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
     <mergeCell ref="K14:M14"/>
     <mergeCell ref="K15:M15"/>
     <mergeCell ref="K16:M16"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H12:J12"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="H15:J15"/>
@@ -2108,6 +2260,20 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="K10:M10"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>